<commit_message>
add two test case in bin.test.js, and modified the excel test_collection file
</commit_message>
<xml_diff>
--- a/Test_collection.xlsx
+++ b/Test_collection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Máy tính\Web_KTPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2DDF6-8C44-4D4C-8764-31584A8C6C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC9C7E-A4C3-4197-968A-394C5F23ECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40832E2C-F3B8-444B-9C9D-48451F9EB369}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Summary</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Tested</t>
   </si>
   <si>
-    <t>Ready for test</t>
-  </si>
-  <si>
     <t>Implementer: Nguyễn Văn Bin</t>
   </si>
   <si>
@@ -106,7 +103,16 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>4.2 - 6</t>
+  </si>
+  <si>
+    <t>Check if the password of client account has encrypted in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open the database -&gt; take 5 random client account </t>
+  </si>
+  <si>
+    <t>password has been encrypted</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,12 +174,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,19 +204,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C49F517-203B-40D8-9923-3844E40156A5}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,20 +549,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -606,10 +603,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>9</v>
@@ -639,6 +636,32 @@
       </c>
       <c r="H8" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -671,20 +694,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -725,7 +748,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="2"/>
     </row>
   </sheetData>
@@ -758,22 +781,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -814,7 +837,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix test case description
</commit_message>
<xml_diff>
--- a/Test_collection.xlsx
+++ b/Test_collection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\OneDrive\Máy tính\Web_KTPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC9C7E-A4C3-4197-968A-394C5F23ECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB43EDBD-83FC-4446-8D75-D0DFF020C334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40832E2C-F3B8-444B-9C9D-48451F9EB369}"/>
   </bookViews>
@@ -55,39 +55,15 @@
     <t>4.2 - 3</t>
   </si>
   <si>
-    <t>does Function throw back full information of the product ?</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>corespond product page with it's information appear</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> click to the picture of any  item.</t>
-  </si>
-  <si>
     <t>4.2 - 5</t>
   </si>
   <si>
-    <t>Check if the account and password of client fill in the login page is quailified</t>
-  </si>
-  <si>
-    <t>Client has to fill the Login form</t>
-  </si>
-  <si>
-    <t>Open the Login Form on the nav bar -&gt; Fill the informaion in the form -&gt; click Login button</t>
-  </si>
-  <si>
-    <t>Client should not be logged if the account is wrong.</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>Account must be right before checking password, if not the app gonna be crash</t>
-  </si>
-  <si>
     <t>Tested</t>
   </si>
   <si>
@@ -106,13 +82,37 @@
     <t>4.2 - 6</t>
   </si>
   <si>
-    <t>Check if the password of client account has encrypted in the database</t>
-  </si>
-  <si>
     <t xml:space="preserve">Open the database -&gt; take 5 random client account </t>
   </si>
   <si>
-    <t>password has been encrypted</t>
+    <t>Hàm có trả về đầy đủ thông tin của cuốn sách hay không ?</t>
+  </si>
+  <si>
+    <t>nhấn chuột vào ảnh của bất kì cuốn sách nào hiện trong trang chủ và trang danh mục</t>
+  </si>
+  <si>
+    <t>Thông tin tương ứng của cuốn sách đó được trả về</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiểm tra tài khoản và mật khẩu và người dùng nhập trong form đăng nhập </t>
+  </si>
+  <si>
+    <t xml:space="preserve">form đăng nhập phải được nhập đầy đủ </t>
+  </si>
+  <si>
+    <t>mở form đăng nhập trên thanh điều hướng -&gt; điền đầy đủ tài khoản và mật khấu -&gt; nhấn nút "Đăng nhập"</t>
+  </si>
+  <si>
+    <t>người dùng vào được tài khoản đã được đăng ký. Nếu tài khoảng chưa đăng kí thì hiện thông báo cho người dùng</t>
+  </si>
+  <si>
+    <t>kiểm tra mật khảu tài khoản người dùng có được mã hóa khi lưu vào cơ sở dữ liệu không ?</t>
+  </si>
+  <si>
+    <t>mật khẩu thực tế phải khác so với trong cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>mật khẩu đã được mã hóa</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C49F517-203B-40D8-9923-3844E40156A5}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,7 +542,7 @@
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="20.77734375" customWidth="1"/>
@@ -550,7 +550,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -562,7 +562,7 @@
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -591,77 +591,77 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +695,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -782,7 +782,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -796,7 +796,7 @@
     </row>
     <row r="6" spans="1:8" s="3" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>

</xml_diff>